<commit_message>
Fix cucumber and rspec tests
</commit_message>
<xml_diff>
--- a/spec/fixtures/HistoricalReport.xlsx
+++ b/spec/fixtures/HistoricalReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelly\Documents\CSCE606_DEADPOOL\spec\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taige/Developer/FPR-Extraction-Metrics/spec/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B2D940-B688-8E4C-9A57-F994251DFD7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8540" windowHeight="5160"/>
+    <workbookView xWindow="1360" yWindow="460" windowWidth="18640" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Nancy Amato FPR 2012</t>
   </si>
@@ -71,19 +72,13 @@
     <t>CSCE 681</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>CSCE  221 H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -193,9 +188,6 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -225,6 +217,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,483 +499,483 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>2012</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>37</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>4.0599999999999996</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>4.04</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>3.58</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>3.68</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>2012</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>20</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>4.21</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>3.78</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="6">
         <v>4</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>2.87</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>2011</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>20</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>3.9924999999999997</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>4.18</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="9">
         <v>3.6320000000000001</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="9">
         <v>3.5640000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>2011</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>42</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>3.8487499999999999</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>4.18</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9">
+        <v>3.6320000000000001</v>
+      </c>
+      <c r="H6" s="9">
+        <v>3.5640000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="10">
-        <v>3.5640000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>2011</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>14</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>3.75</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>3.68</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="9">
         <v>4</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <v>2.6960000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>2011</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>57</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>3.79</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>4.1100000000000003</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="10">
+      <c r="G8" s="9">
+        <v>4</v>
+      </c>
+      <c r="H8" s="9">
         <v>3.7469999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-    </row>
-    <row r="16" spans="1:8" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="14"/>
-    </row>
-    <row r="20" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
+    <row r="9" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+    </row>
+    <row r="14" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+    </row>
+    <row r="15" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>